<commit_message>
buildings for BC EMH project
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_market share limits/formula_CIMS_market share limits_ON.xlsx
+++ b/csv/model/CIMS_market share limits/formula_CIMS_market share limits_ON.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_market share limits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EFF5521-0A4C-438B-A2DC-D728D53B32D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F6EE5C2-B0E9-436D-B831-817767B35631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35835" yWindow="4365" windowWidth="17250" windowHeight="8865" xr2:uid="{5B54CF6C-552B-4A01-80A2-CE7041CE23F4}"/>
+    <workbookView xWindow="37170" yWindow="5385" windowWidth="17250" windowHeight="8865" xr2:uid="{AFAA18D1-7240-42EF-89E9-AFB80A8B230B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="295">
   <si>
     <t>&lt;-- Navigate by typing to search</t>
   </si>
@@ -837,57 +837,6 @@
   </si>
   <si>
     <t>Eff wood waste</t>
-  </si>
-  <si>
-    <t>CIMS.CAN.ON.Residential.Buildings.Ranges</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Ranges</t>
-  </si>
-  <si>
-    <t>NG existing</t>
-  </si>
-  <si>
-    <t>CIMS.CAN.ON.Residential.Buildings.Non-appliance Hot Water</t>
-  </si>
-  <si>
-    <t>Non-appliance Hot Water</t>
-  </si>
-  <si>
-    <t>Low flow devices</t>
-  </si>
-  <si>
-    <t>CIMS.CAN.ON.Residential.Space Heating</t>
-  </si>
-  <si>
-    <t>Wood stove efficient</t>
-  </si>
-  <si>
-    <t>CIMS.CAN.ON.Residential.Clothes Drying.Machine</t>
-  </si>
-  <si>
-    <t>Machine</t>
-  </si>
-  <si>
-    <t>NG Std</t>
-  </si>
-  <si>
-    <t>NG heat pump</t>
-  </si>
-  <si>
-    <t>Retrofit_new_max</t>
-  </si>
-  <si>
-    <t>CIMS.CAN.ON.Residential.Water Heating.House</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Oil existing</t>
   </si>
   <si>
     <t>CIMS.CAN.ON.Transportation Personal.Transit.Public Bus</t>
@@ -1342,11 +1291,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5901AB40-6804-4A20-9E88-EBA31C8F381C}">
-  <dimension ref="A1:X251"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3762CA1B-7500-4B1F-82E0-C143DB7CDD6F}">
+  <dimension ref="A1:X242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X251"/>
+      <selection sqref="A1:X242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14528,7 +14477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>259</v>
       </c>
@@ -14587,7 +14536,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>262</v>
       </c>
@@ -14646,7 +14595,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>262</v>
       </c>
@@ -14705,7 +14654,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>262</v>
       </c>
@@ -14764,7 +14713,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>267</v>
       </c>
@@ -14790,40 +14739,40 @@
         <v>20</v>
       </c>
       <c r="M229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="N229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="O229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="P229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="Q229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="R229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="S229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="T229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="U229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="V229">
-        <v>0.15</v>
+        <v>1E-3</v>
       </c>
       <c r="W229">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>271</v>
       </c>
@@ -14843,19 +14792,19 @@
         <v>273</v>
       </c>
       <c r="G230" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="L230" t="s">
         <v>20</v>
       </c>
       <c r="M230">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="N230">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="O230">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="P230">
         <v>1</v>
@@ -14882,7 +14831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>274</v>
       </c>
@@ -14893,13 +14842,13 @@
         <v>15</v>
       </c>
       <c r="D231" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="E231" t="s">
-        <v>98</v>
+        <v>276</v>
       </c>
       <c r="F231" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="G231" t="s">
         <v>19</v>
@@ -14908,42 +14857,42 @@
         <v>20</v>
       </c>
       <c r="M231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="N231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="O231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="P231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="Q231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="R231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="S231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="T231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="U231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="V231">
-        <v>2.7E-2</v>
+        <v>0.56385600000000002</v>
       </c>
       <c r="W231">
-        <v>2.7E-2</v>
-      </c>
-    </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.56385600000000002</v>
+      </c>
+    </row>
+    <row r="232" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B232" t="s">
         <v>5</v>
@@ -14952,57 +14901,57 @@
         <v>15</v>
       </c>
       <c r="D232" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="E232" t="s">
-        <v>98</v>
+        <v>280</v>
       </c>
       <c r="F232" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="G232" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L232" t="s">
         <v>20</v>
       </c>
       <c r="M232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="N232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="O232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="P232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="Q232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="R232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="S232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="T232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="U232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="V232">
-        <v>2.5999999999999999E-2</v>
+        <v>0.95</v>
       </c>
       <c r="W232">
-        <v>2.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="233" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="B233" t="s">
         <v>5</v>
@@ -15011,13 +14960,13 @@
         <v>15</v>
       </c>
       <c r="D233" t="s">
-        <v>268</v>
+        <v>16</v>
       </c>
       <c r="E233" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F233" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G233" t="s">
         <v>19</v>
@@ -15026,52 +14975,45 @@
         <v>20</v>
       </c>
       <c r="M233">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="N233">
-        <f t="shared" ref="N233:W236" si="0">M233</f>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="O233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="P233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="Q233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="R233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="S233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="T233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="U233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="V233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="W233">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+      <c r="X233" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="234" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="B234" t="s">
         <v>5</v>
@@ -15080,13 +15022,13 @@
         <v>15</v>
       </c>
       <c r="D234" t="s">
-        <v>268</v>
+        <v>26</v>
       </c>
       <c r="E234" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F234" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G234" t="s">
         <v>19</v>
@@ -15095,52 +15037,45 @@
         <v>20</v>
       </c>
       <c r="M234">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="N234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="O234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="P234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="Q234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="R234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="S234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="T234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="U234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="V234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="W234">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+      <c r="X234" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="235" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B235" t="s">
         <v>5</v>
@@ -15149,67 +15084,60 @@
         <v>15</v>
       </c>
       <c r="D235" t="s">
-        <v>268</v>
+        <v>36</v>
       </c>
       <c r="E235" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F235" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G235" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
       <c r="L235" t="s">
         <v>20</v>
       </c>
       <c r="M235">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="N235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="O235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="P235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Q235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="T235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V235">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="W235">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+      <c r="X235" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="236" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B236" t="s">
         <v>5</v>
@@ -15218,67 +15146,60 @@
         <v>15</v>
       </c>
       <c r="D236" t="s">
-        <v>268</v>
+        <v>78</v>
       </c>
       <c r="E236" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F236" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G236" t="s">
-        <v>280</v>
+        <v>19</v>
       </c>
       <c r="L236" t="s">
         <v>20</v>
       </c>
       <c r="M236">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="N236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="O236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="P236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="Q236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="R236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="T236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V236">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="W236">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+      <c r="X236" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="237" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="B237" t="s">
         <v>5</v>
@@ -15287,116 +15208,122 @@
         <v>15</v>
       </c>
       <c r="D237" t="s">
-        <v>268</v>
+        <v>102</v>
       </c>
       <c r="E237" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F237" t="s">
+        <v>284</v>
+      </c>
+      <c r="G237" t="s">
+        <v>19</v>
+      </c>
+      <c r="L237" t="s">
+        <v>20</v>
+      </c>
+      <c r="M237">
+        <v>0.01</v>
+      </c>
+      <c r="N237">
+        <v>0.01</v>
+      </c>
+      <c r="O237">
+        <v>0.01</v>
+      </c>
+      <c r="P237">
+        <v>0.01</v>
+      </c>
+      <c r="Q237">
+        <v>0.01</v>
+      </c>
+      <c r="R237">
+        <v>0.01</v>
+      </c>
+      <c r="S237">
+        <v>0.01</v>
+      </c>
+      <c r="T237">
+        <v>0.01</v>
+      </c>
+      <c r="U237">
+        <v>0.01</v>
+      </c>
+      <c r="V237">
+        <v>0.01</v>
+      </c>
+      <c r="W237">
+        <v>0.01</v>
+      </c>
+      <c r="X237" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="238" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>290</v>
+      </c>
+      <c r="B238" t="s">
+        <v>5</v>
+      </c>
+      <c r="C238" t="s">
+        <v>15</v>
+      </c>
+      <c r="D238" t="s">
+        <v>133</v>
+      </c>
+      <c r="E238" t="s">
         <v>283</v>
       </c>
-      <c r="G237" t="s">
-        <v>19</v>
-      </c>
-      <c r="L237" t="s">
-        <v>20</v>
-      </c>
-      <c r="M237">
-        <v>0.03</v>
-      </c>
-      <c r="N237">
-        <v>0.03</v>
-      </c>
-      <c r="O237">
-        <v>0.03</v>
-      </c>
-      <c r="P237">
-        <v>0.03</v>
-      </c>
-      <c r="Q237">
-        <v>0.03</v>
-      </c>
-      <c r="R237">
-        <v>0.03</v>
-      </c>
-      <c r="S237">
-        <v>0.03</v>
-      </c>
-      <c r="T237">
-        <v>0.03</v>
-      </c>
-      <c r="U237">
-        <v>0.03</v>
-      </c>
-      <c r="V237">
-        <v>0.03</v>
-      </c>
-      <c r="W237">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A238" t="s">
+      <c r="F238" t="s">
         <v>284</v>
       </c>
-      <c r="B238" t="s">
-        <v>5</v>
-      </c>
-      <c r="C238" t="s">
-        <v>15</v>
-      </c>
-      <c r="D238" t="s">
+      <c r="G238" t="s">
+        <v>19</v>
+      </c>
+      <c r="L238" t="s">
+        <v>20</v>
+      </c>
+      <c r="M238">
+        <v>0.01</v>
+      </c>
+      <c r="N238">
+        <v>0.01</v>
+      </c>
+      <c r="O238">
+        <v>0.01</v>
+      </c>
+      <c r="P238">
+        <v>0.01</v>
+      </c>
+      <c r="Q238">
+        <v>0.01</v>
+      </c>
+      <c r="R238">
+        <v>0.01</v>
+      </c>
+      <c r="S238">
+        <v>0.01</v>
+      </c>
+      <c r="T238">
+        <v>0.01</v>
+      </c>
+      <c r="U238">
+        <v>0.01</v>
+      </c>
+      <c r="V238">
+        <v>0.01</v>
+      </c>
+      <c r="W238">
+        <v>0.01</v>
+      </c>
+      <c r="X238" t="s">
         <v>285</v>
       </c>
-      <c r="E238" t="s">
-        <v>286</v>
-      </c>
-      <c r="F238" t="s">
-        <v>287</v>
-      </c>
-      <c r="G238" t="s">
-        <v>19</v>
-      </c>
-      <c r="L238" t="s">
-        <v>20</v>
-      </c>
-      <c r="M238">
-        <v>1E-3</v>
-      </c>
-      <c r="N238">
-        <v>1E-3</v>
-      </c>
-      <c r="O238">
-        <v>1E-3</v>
-      </c>
-      <c r="P238">
-        <v>1E-3</v>
-      </c>
-      <c r="Q238">
-        <v>1E-3</v>
-      </c>
-      <c r="R238">
-        <v>1E-3</v>
-      </c>
-      <c r="S238">
-        <v>1E-3</v>
-      </c>
-      <c r="T238">
-        <v>1E-3</v>
-      </c>
-      <c r="U238">
-        <v>1E-3</v>
-      </c>
-      <c r="V238">
-        <v>1E-3</v>
-      </c>
-      <c r="W238">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="239" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B239" t="s">
         <v>5</v>
@@ -15405,57 +15332,60 @@
         <v>15</v>
       </c>
       <c r="D239" t="s">
+        <v>169</v>
+      </c>
+      <c r="E239" t="s">
+        <v>283</v>
+      </c>
+      <c r="F239" t="s">
+        <v>284</v>
+      </c>
+      <c r="G239" t="s">
+        <v>19</v>
+      </c>
+      <c r="L239" t="s">
+        <v>20</v>
+      </c>
+      <c r="M239">
+        <v>0.01</v>
+      </c>
+      <c r="N239">
+        <v>0.01</v>
+      </c>
+      <c r="O239">
+        <v>0.01</v>
+      </c>
+      <c r="P239">
+        <v>0.01</v>
+      </c>
+      <c r="Q239">
+        <v>0.01</v>
+      </c>
+      <c r="R239">
+        <v>0.01</v>
+      </c>
+      <c r="S239">
+        <v>0.01</v>
+      </c>
+      <c r="T239">
+        <v>0.01</v>
+      </c>
+      <c r="U239">
+        <v>0.01</v>
+      </c>
+      <c r="V239">
+        <v>0.01</v>
+      </c>
+      <c r="W239">
+        <v>0.01</v>
+      </c>
+      <c r="X239" t="s">
         <v>285</v>
       </c>
-      <c r="E239" t="s">
-        <v>289</v>
-      </c>
-      <c r="F239" t="s">
-        <v>290</v>
-      </c>
-      <c r="G239" t="s">
-        <v>33</v>
-      </c>
-      <c r="L239" t="s">
-        <v>20</v>
-      </c>
-      <c r="M239">
-        <v>1</v>
-      </c>
-      <c r="N239">
-        <v>1</v>
-      </c>
-      <c r="O239">
-        <v>1</v>
-      </c>
-      <c r="P239">
-        <v>1</v>
-      </c>
-      <c r="Q239">
-        <v>1</v>
-      </c>
-      <c r="R239">
-        <v>1</v>
-      </c>
-      <c r="S239">
-        <v>1</v>
-      </c>
-      <c r="T239">
-        <v>1</v>
-      </c>
-      <c r="U239">
-        <v>1</v>
-      </c>
-      <c r="V239">
-        <v>1</v>
-      </c>
-      <c r="W239">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.3">
+    </row>
+    <row r="240" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B240" t="s">
         <v>5</v>
@@ -15464,13 +15394,13 @@
         <v>15</v>
       </c>
       <c r="D240" t="s">
-        <v>292</v>
+        <v>192</v>
       </c>
       <c r="E240" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="F240" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="G240" t="s">
         <v>19</v>
@@ -15479,42 +15409,45 @@
         <v>20</v>
       </c>
       <c r="M240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="N240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="O240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="P240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="Q240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="R240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="S240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="T240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="U240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="V240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
       </c>
       <c r="W240">
-        <v>0.56385600000000002</v>
+        <v>0.01</v>
+      </c>
+      <c r="X240" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="241" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B241" t="s">
         <v>5</v>
@@ -15523,13 +15456,13 @@
         <v>15</v>
       </c>
       <c r="D241" t="s">
-        <v>296</v>
+        <v>216</v>
       </c>
       <c r="E241" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="F241" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="G241" t="s">
         <v>19</v>
@@ -15538,42 +15471,45 @@
         <v>20</v>
       </c>
       <c r="M241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="N241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="O241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="P241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="Q241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="R241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="S241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="T241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="U241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="V241">
-        <v>0.95</v>
+        <v>0.01</v>
       </c>
       <c r="W241">
-        <v>0.95</v>
+        <v>0.01</v>
+      </c>
+      <c r="X241" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="242" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B242" t="s">
         <v>5</v>
@@ -15582,13 +15518,13 @@
         <v>15</v>
       </c>
       <c r="D242" t="s">
-        <v>16</v>
+        <v>257</v>
       </c>
       <c r="E242" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="F242" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="G242" t="s">
         <v>19</v>
@@ -15630,565 +15566,7 @@
         <v>0.01</v>
       </c>
       <c r="X242" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A243" t="s">
-        <v>303</v>
-      </c>
-      <c r="B243" t="s">
-        <v>5</v>
-      </c>
-      <c r="C243" t="s">
-        <v>15</v>
-      </c>
-      <c r="D243" t="s">
-        <v>26</v>
-      </c>
-      <c r="E243" t="s">
-        <v>300</v>
-      </c>
-      <c r="F243" t="s">
-        <v>301</v>
-      </c>
-      <c r="G243" t="s">
-        <v>19</v>
-      </c>
-      <c r="L243" t="s">
-        <v>20</v>
-      </c>
-      <c r="M243">
-        <v>0.01</v>
-      </c>
-      <c r="N243">
-        <v>0.01</v>
-      </c>
-      <c r="O243">
-        <v>0.01</v>
-      </c>
-      <c r="P243">
-        <v>0.01</v>
-      </c>
-      <c r="Q243">
-        <v>0.01</v>
-      </c>
-      <c r="R243">
-        <v>0.01</v>
-      </c>
-      <c r="S243">
-        <v>0.01</v>
-      </c>
-      <c r="T243">
-        <v>0.01</v>
-      </c>
-      <c r="U243">
-        <v>0.01</v>
-      </c>
-      <c r="V243">
-        <v>0.01</v>
-      </c>
-      <c r="W243">
-        <v>0.01</v>
-      </c>
-      <c r="X243" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A244" t="s">
-        <v>304</v>
-      </c>
-      <c r="B244" t="s">
-        <v>5</v>
-      </c>
-      <c r="C244" t="s">
-        <v>15</v>
-      </c>
-      <c r="D244" t="s">
-        <v>36</v>
-      </c>
-      <c r="E244" t="s">
-        <v>300</v>
-      </c>
-      <c r="F244" t="s">
-        <v>301</v>
-      </c>
-      <c r="G244" t="s">
-        <v>19</v>
-      </c>
-      <c r="L244" t="s">
-        <v>20</v>
-      </c>
-      <c r="M244">
-        <v>0.01</v>
-      </c>
-      <c r="N244">
-        <v>0.01</v>
-      </c>
-      <c r="O244">
-        <v>0.01</v>
-      </c>
-      <c r="P244">
-        <v>0.01</v>
-      </c>
-      <c r="Q244">
-        <v>0.01</v>
-      </c>
-      <c r="R244">
-        <v>0.01</v>
-      </c>
-      <c r="S244">
-        <v>0.01</v>
-      </c>
-      <c r="T244">
-        <v>0.01</v>
-      </c>
-      <c r="U244">
-        <v>0.01</v>
-      </c>
-      <c r="V244">
-        <v>0.01</v>
-      </c>
-      <c r="W244">
-        <v>0.01</v>
-      </c>
-      <c r="X244" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
-        <v>305</v>
-      </c>
-      <c r="B245" t="s">
-        <v>5</v>
-      </c>
-      <c r="C245" t="s">
-        <v>15</v>
-      </c>
-      <c r="D245" t="s">
-        <v>78</v>
-      </c>
-      <c r="E245" t="s">
-        <v>300</v>
-      </c>
-      <c r="F245" t="s">
-        <v>301</v>
-      </c>
-      <c r="G245" t="s">
-        <v>19</v>
-      </c>
-      <c r="L245" t="s">
-        <v>20</v>
-      </c>
-      <c r="M245">
-        <v>0.01</v>
-      </c>
-      <c r="N245">
-        <v>0.01</v>
-      </c>
-      <c r="O245">
-        <v>0.01</v>
-      </c>
-      <c r="P245">
-        <v>0.01</v>
-      </c>
-      <c r="Q245">
-        <v>0.01</v>
-      </c>
-      <c r="R245">
-        <v>0.01</v>
-      </c>
-      <c r="S245">
-        <v>0.01</v>
-      </c>
-      <c r="T245">
-        <v>0.01</v>
-      </c>
-      <c r="U245">
-        <v>0.01</v>
-      </c>
-      <c r="V245">
-        <v>0.01</v>
-      </c>
-      <c r="W245">
-        <v>0.01</v>
-      </c>
-      <c r="X245" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A246" t="s">
-        <v>306</v>
-      </c>
-      <c r="B246" t="s">
-        <v>5</v>
-      </c>
-      <c r="C246" t="s">
-        <v>15</v>
-      </c>
-      <c r="D246" t="s">
-        <v>102</v>
-      </c>
-      <c r="E246" t="s">
-        <v>300</v>
-      </c>
-      <c r="F246" t="s">
-        <v>301</v>
-      </c>
-      <c r="G246" t="s">
-        <v>19</v>
-      </c>
-      <c r="L246" t="s">
-        <v>20</v>
-      </c>
-      <c r="M246">
-        <v>0.01</v>
-      </c>
-      <c r="N246">
-        <v>0.01</v>
-      </c>
-      <c r="O246">
-        <v>0.01</v>
-      </c>
-      <c r="P246">
-        <v>0.01</v>
-      </c>
-      <c r="Q246">
-        <v>0.01</v>
-      </c>
-      <c r="R246">
-        <v>0.01</v>
-      </c>
-      <c r="S246">
-        <v>0.01</v>
-      </c>
-      <c r="T246">
-        <v>0.01</v>
-      </c>
-      <c r="U246">
-        <v>0.01</v>
-      </c>
-      <c r="V246">
-        <v>0.01</v>
-      </c>
-      <c r="W246">
-        <v>0.01</v>
-      </c>
-      <c r="X246" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
-        <v>307</v>
-      </c>
-      <c r="B247" t="s">
-        <v>5</v>
-      </c>
-      <c r="C247" t="s">
-        <v>15</v>
-      </c>
-      <c r="D247" t="s">
-        <v>133</v>
-      </c>
-      <c r="E247" t="s">
-        <v>300</v>
-      </c>
-      <c r="F247" t="s">
-        <v>301</v>
-      </c>
-      <c r="G247" t="s">
-        <v>19</v>
-      </c>
-      <c r="L247" t="s">
-        <v>20</v>
-      </c>
-      <c r="M247">
-        <v>0.01</v>
-      </c>
-      <c r="N247">
-        <v>0.01</v>
-      </c>
-      <c r="O247">
-        <v>0.01</v>
-      </c>
-      <c r="P247">
-        <v>0.01</v>
-      </c>
-      <c r="Q247">
-        <v>0.01</v>
-      </c>
-      <c r="R247">
-        <v>0.01</v>
-      </c>
-      <c r="S247">
-        <v>0.01</v>
-      </c>
-      <c r="T247">
-        <v>0.01</v>
-      </c>
-      <c r="U247">
-        <v>0.01</v>
-      </c>
-      <c r="V247">
-        <v>0.01</v>
-      </c>
-      <c r="W247">
-        <v>0.01</v>
-      </c>
-      <c r="X247" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A248" t="s">
-        <v>308</v>
-      </c>
-      <c r="B248" t="s">
-        <v>5</v>
-      </c>
-      <c r="C248" t="s">
-        <v>15</v>
-      </c>
-      <c r="D248" t="s">
-        <v>169</v>
-      </c>
-      <c r="E248" t="s">
-        <v>300</v>
-      </c>
-      <c r="F248" t="s">
-        <v>301</v>
-      </c>
-      <c r="G248" t="s">
-        <v>19</v>
-      </c>
-      <c r="L248" t="s">
-        <v>20</v>
-      </c>
-      <c r="M248">
-        <v>0.01</v>
-      </c>
-      <c r="N248">
-        <v>0.01</v>
-      </c>
-      <c r="O248">
-        <v>0.01</v>
-      </c>
-      <c r="P248">
-        <v>0.01</v>
-      </c>
-      <c r="Q248">
-        <v>0.01</v>
-      </c>
-      <c r="R248">
-        <v>0.01</v>
-      </c>
-      <c r="S248">
-        <v>0.01</v>
-      </c>
-      <c r="T248">
-        <v>0.01</v>
-      </c>
-      <c r="U248">
-        <v>0.01</v>
-      </c>
-      <c r="V248">
-        <v>0.01</v>
-      </c>
-      <c r="W248">
-        <v>0.01</v>
-      </c>
-      <c r="X248" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>309</v>
-      </c>
-      <c r="B249" t="s">
-        <v>5</v>
-      </c>
-      <c r="C249" t="s">
-        <v>15</v>
-      </c>
-      <c r="D249" t="s">
-        <v>192</v>
-      </c>
-      <c r="E249" t="s">
-        <v>300</v>
-      </c>
-      <c r="F249" t="s">
-        <v>301</v>
-      </c>
-      <c r="G249" t="s">
-        <v>19</v>
-      </c>
-      <c r="L249" t="s">
-        <v>20</v>
-      </c>
-      <c r="M249">
-        <v>0.01</v>
-      </c>
-      <c r="N249">
-        <v>0.01</v>
-      </c>
-      <c r="O249">
-        <v>0.01</v>
-      </c>
-      <c r="P249">
-        <v>0.01</v>
-      </c>
-      <c r="Q249">
-        <v>0.01</v>
-      </c>
-      <c r="R249">
-        <v>0.01</v>
-      </c>
-      <c r="S249">
-        <v>0.01</v>
-      </c>
-      <c r="T249">
-        <v>0.01</v>
-      </c>
-      <c r="U249">
-        <v>0.01</v>
-      </c>
-      <c r="V249">
-        <v>0.01</v>
-      </c>
-      <c r="W249">
-        <v>0.01</v>
-      </c>
-      <c r="X249" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A250" t="s">
-        <v>310</v>
-      </c>
-      <c r="B250" t="s">
-        <v>5</v>
-      </c>
-      <c r="C250" t="s">
-        <v>15</v>
-      </c>
-      <c r="D250" t="s">
-        <v>216</v>
-      </c>
-      <c r="E250" t="s">
-        <v>300</v>
-      </c>
-      <c r="F250" t="s">
-        <v>301</v>
-      </c>
-      <c r="G250" t="s">
-        <v>19</v>
-      </c>
-      <c r="L250" t="s">
-        <v>20</v>
-      </c>
-      <c r="M250">
-        <v>0.01</v>
-      </c>
-      <c r="N250">
-        <v>0.01</v>
-      </c>
-      <c r="O250">
-        <v>0.01</v>
-      </c>
-      <c r="P250">
-        <v>0.01</v>
-      </c>
-      <c r="Q250">
-        <v>0.01</v>
-      </c>
-      <c r="R250">
-        <v>0.01</v>
-      </c>
-      <c r="S250">
-        <v>0.01</v>
-      </c>
-      <c r="T250">
-        <v>0.01</v>
-      </c>
-      <c r="U250">
-        <v>0.01</v>
-      </c>
-      <c r="V250">
-        <v>0.01</v>
-      </c>
-      <c r="W250">
-        <v>0.01</v>
-      </c>
-      <c r="X250" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A251" t="s">
-        <v>311</v>
-      </c>
-      <c r="B251" t="s">
-        <v>5</v>
-      </c>
-      <c r="C251" t="s">
-        <v>15</v>
-      </c>
-      <c r="D251" t="s">
-        <v>257</v>
-      </c>
-      <c r="E251" t="s">
-        <v>300</v>
-      </c>
-      <c r="F251" t="s">
-        <v>301</v>
-      </c>
-      <c r="G251" t="s">
-        <v>19</v>
-      </c>
-      <c r="L251" t="s">
-        <v>20</v>
-      </c>
-      <c r="M251">
-        <v>0.01</v>
-      </c>
-      <c r="N251">
-        <v>0.01</v>
-      </c>
-      <c r="O251">
-        <v>0.01</v>
-      </c>
-      <c r="P251">
-        <v>0.01</v>
-      </c>
-      <c r="Q251">
-        <v>0.01</v>
-      </c>
-      <c r="R251">
-        <v>0.01</v>
-      </c>
-      <c r="S251">
-        <v>0.01</v>
-      </c>
-      <c r="T251">
-        <v>0.01</v>
-      </c>
-      <c r="U251">
-        <v>0.01</v>
-      </c>
-      <c r="V251">
-        <v>0.01</v>
-      </c>
-      <c r="W251">
-        <v>0.01</v>
-      </c>
-      <c r="X251" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>